<commit_message>
Wheat cut and growth
</commit_message>
<xml_diff>
--- a/Тайминг.xlsx
+++ b/Тайминг.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="15255" windowHeight="8715" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="15255" windowHeight="8715"/>
   </bookViews>
   <sheets>
     <sheet name="Тайминг" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Дата</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>часть</t>
+  </si>
+  <si>
+    <t>Косить пшеницу</t>
+  </si>
+  <si>
+    <t>Требует доработки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 час </t>
+  </si>
+  <si>
+    <t>Проверить коллайдер (не выключается)</t>
   </si>
 </sst>
 </file>
@@ -694,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -703,7 +715,7 @@
     <col min="1" max="1" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -894,39 +906,73 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="10"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="5">
+        <v>45002</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="10"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="8"/>
+      <c r="A17" s="5">
+        <v>45003</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="10"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="8"/>
+      <c r="C18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="10"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="8"/>
+      <c r="A19" s="5">
+        <v>45004</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="10"/>
       <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="10"/>
       <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4">
@@ -961,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>